<commit_message>
Goshop 13st Commit Rev 1.0
</commit_message>
<xml_diff>
--- a/liusming@hotmail.com/sales.xlsx
+++ b/liusming@hotmail.com/sales.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="銷售記錄" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="銷售總合" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -682,17 +684,249 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-03-09</t>
+          <t>2025-03-12</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>625.28</v>
+        <v>794.4100000000001</v>
       </c>
       <c r="C16" t="n">
-        <v>62.7</v>
+        <v>79.60999999999999</v>
       </c>
       <c r="D16" t="n">
-        <v>562.5799999999999</v>
+        <v>714.8000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>檔案名</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>revenue</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250214.xlsx</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>412.2200000000001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250215.xlsx</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>201.18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250217.xlsx</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>252.46</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250218.xlsx</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>286.16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250219_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>155.76</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250220_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>270.26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250221_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>195.84</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250223_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>476.4399999999999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250225_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>349.35</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250226_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>316.3099999999999</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250227_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>319.52</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250228_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>145.4399999999999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250301_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>278.08</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250302_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>196.36</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250303_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>263.1799999999999</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250305_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>644.8000000000001</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>goshop_orders_20250312_liusming@hotmail.com.xlsx</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>714.8000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>總收入</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>5478.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>